<commit_message>
isDeleted added to flooringCoating.js in models
</commit_message>
<xml_diff>
--- a/_docs/ref/jce_calcs.xlsx
+++ b/_docs/ref/jce_calcs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44563\cge\_docs\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nw_webapps_2017_spring\_docs\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -935,14 +935,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,7 +1318,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42824.682683101855</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42824.682683101855</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3337,10 +3337,10 @@
       <c r="C22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="61"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3355,10 +3355,10 @@
       <c r="D23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E23" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="59"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3367,10 +3367,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="59"/>
+      <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4740,11 +4740,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4752,6 +4747,11 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42824.682683101855</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changed Team names in About page
</commit_message>
<xml_diff>
--- a/_docs/ref/jce_calcs.xlsx
+++ b/_docs/ref/jce_calcs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -935,14 +935,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,8 +1318,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42824.682683101855</v>
+        <v>42824.699191666667</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42824.682683101855</v>
+        <v>42824.699191666667</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3337,10 +3337,10 @@
       <c r="C22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="60"/>
+      <c r="F22" s="61"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3355,10 +3355,10 @@
       <c r="D23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="61"/>
+      <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3367,10 +3367,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="61"/>
+      <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4740,6 +4740,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4747,11 +4752,6 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42824.682683101855</v>
+        <v>42824.699191666667</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6572,8 +6572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
After changing topcoats to T with issue 43
</commit_message>
<xml_diff>
--- a/_docs/ref/jce_calcs.xlsx
+++ b/_docs/ref/jce_calcs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44563\cge\_docs\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528802\Desktop\cge\_docs\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -935,14 +935,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,7 +1318,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42828.570116319446</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3002,8 +3002,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N70" sqref="N70"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42828.570116319446</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3337,10 +3337,10 @@
       <c r="C22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="60" t="s">
+      <c r="E22" s="59" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="61"/>
+      <c r="F22" s="60"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3355,10 +3355,10 @@
       <c r="D23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="59" t="s">
+      <c r="E23" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="59"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3367,10 +3367,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="59" t="s">
+      <c r="E24" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="59"/>
+      <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4740,11 +4740,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4752,6 +4747,11 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42821.912740624997</v>
+        <v>42828.570116319446</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
changes to delete, edit buttons
</commit_message>
<xml_diff>
--- a/_docs/ref/jce_calcs.xlsx
+++ b/_docs/ref/jce_calcs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528802\Desktop\cge\_docs\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nw_webapps_2017_spring\cge\_docs\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -935,14 +935,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.748572337965</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3002,7 +3002,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.748572337965</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3337,10 +3337,10 @@
       <c r="C22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="60"/>
+      <c r="F22" s="61"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3355,10 +3355,10 @@
       <c r="D23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="61"/>
+      <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3367,10 +3367,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="61"/>
+      <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4740,6 +4740,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4747,11 +4752,6 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4769,8 +4769,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.748572337965</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added max min values in views/floaringcoatings/create.ejs page for aggregated products
</commit_message>
<xml_diff>
--- a/_docs/ref/jce_calcs.xlsx
+++ b/_docs/ref/jce_calcs.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s528802\Desktop\cge\_docs\ref\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cge\_docs\ref\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="2"/>
+    <workbookView minimized="1" xWindow="-15" yWindow="-15" windowWidth="21810" windowHeight="11640" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="8" r:id="rId1"/>
@@ -935,14 +935,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1318,8 +1318,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R96"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+    <sheetView showGridLines="0" topLeftCell="B12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.743234374997</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3002,7 +3002,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:R97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
@@ -3123,7 +3123,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.743234374997</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3337,10 +3337,10 @@
       <c r="C22" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="E22" s="59" t="s">
+      <c r="E22" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="60"/>
+      <c r="F22" s="61"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -3355,10 +3355,10 @@
       <c r="D23" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="61" t="s">
+      <c r="E23" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="F23" s="61"/>
+      <c r="F23" s="59"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -3367,10 +3367,10 @@
       <c r="C24" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E24" s="61" t="s">
+      <c r="E24" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="61"/>
+      <c r="F24" s="59"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
@@ -4740,6 +4740,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="C50:C51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
     <mergeCell ref="J50:J51"/>
     <mergeCell ref="K50:K51"/>
     <mergeCell ref="L50:L51"/>
@@ -4747,11 +4752,6 @@
     <mergeCell ref="E24:F24"/>
     <mergeCell ref="H50:H51"/>
     <mergeCell ref="I50:I51"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="50" orientation="landscape" r:id="rId1"/>
@@ -4890,7 +4890,7 @@
       </c>
       <c r="D8" s="36">
         <f ca="1">NOW()</f>
-        <v>42828.570116319446</v>
+        <v>42835.743234374997</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -6572,8 +6572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>